<commit_message>
Updated main.py, Data.xlsx, MasterSheetMaker.py
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -9,11 +9,11 @@
     <sheet name="Master" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Teacher_Input" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Subject_Input" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Teacher_Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Constraints_Input" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Classes" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -99,11 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -118,10 +117,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +472,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -491,8 +495,8 @@
     <col width="10.140625" bestFit="1" customWidth="1" style="1" min="16" max="16"/>
     <col width="11.140625" bestFit="1" customWidth="1" style="1" min="17" max="17"/>
     <col width="13.7109375" bestFit="1" customWidth="1" style="1" min="18" max="18"/>
-    <col width="9.140625" customWidth="1" style="1" min="19" max="21"/>
-    <col width="9.140625" customWidth="1" style="1" min="22" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="19" max="26"/>
+    <col width="9.140625" customWidth="1" style="1" min="27" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="11">
@@ -2269,17 +2273,17 @@
     <row r="24">
       <c r="G24" t="inlineStr">
         <is>
-          <t>T46</t>
+          <t>T49</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>Yoga</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2294,7 +2298,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>140101</t>
+          <t>130101</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -2336,12 +2340,12 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Lib</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2356,7 +2360,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>130101</t>
+          <t>140101</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2393,17 +2397,17 @@
     <row r="26">
       <c r="G26" t="inlineStr">
         <is>
-          <t>T52</t>
+          <t>T46</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Lib</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2418,7 +2422,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>120101</t>
+          <t>140101</t>
         </is>
       </c>
     </row>
@@ -2442,14 +2446,14 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.42578125" customWidth="1" style="3" min="1" max="1"/>
-    <col width="15.28515625" customWidth="1" style="3" min="2" max="2"/>
-    <col width="14.85546875" customWidth="1" style="3" min="3" max="3"/>
+    <col width="13.42578125" customWidth="1" style="13" min="1" max="1"/>
+    <col width="15.28515625" customWidth="1" style="13" min="2" max="2"/>
+    <col width="14.85546875" customWidth="1" style="13" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3434,20 +3438,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18.42578125" customWidth="1" style="13" min="2" max="2"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="3">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="15.75" customHeight="1" s="13">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Subjects</t>
         </is>
       </c>
+      <c r="B1" s="7" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3554,7 +3562,42 @@
         </is>
       </c>
     </row>
-    <row r="17"/>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Hindi</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Marathi</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>GK</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+    </row>
+    <row r="22"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3566,244 +3609,466 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18.42578125" customWidth="1" style="3" min="1" max="1"/>
-    <col width="17.5703125" customWidth="1" style="3" min="2" max="2"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="13" min="2" max="2"/>
+    <col width="7.28515625" customWidth="1" style="13" min="3" max="3"/>
+    <col width="10.140625" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Teacher_Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>200001</v>
+      <c r="B1" s="12" t="inlineStr">
+        <is>
+          <t>Max Lectures/Week</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="13">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Subjects</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
+      <c r="A3">
+        <f>IF(Subject_Input!A2&lt;&gt;"",Subject_Input!A2,"")</f>
+        <v/>
       </c>
       <c r="B3" t="n">
-        <v>200102</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>T3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>200301</v>
+      <c r="A4">
+        <f>IF(Subject_Input!A3&lt;&gt;"",Subject_Input!A3,"")</f>
+        <v/>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>T4</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>200709</v>
+      <c r="A5">
+        <f>IF(Subject_Input!A4&lt;&gt;"",Subject_Input!A4,"")</f>
+        <v/>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>T5</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>200002</v>
+      <c r="A6">
+        <f>IF(Subject_Input!A5&lt;&gt;"",Subject_Input!A5,"")</f>
+        <v/>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>T6</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>200101</v>
+      <c r="A7">
+        <f>IF(Subject_Input!A6&lt;&gt;"",Subject_Input!A6,"")</f>
+        <v/>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>T7</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>200505</v>
+      <c r="A8">
+        <f>IF(Subject_Input!A7&lt;&gt;"",Subject_Input!A7,"")</f>
+        <v/>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>T8</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>200302</v>
+      <c r="A9">
+        <f>IF(Subject_Input!A8&lt;&gt;"",Subject_Input!A8,"")</f>
+        <v/>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>T9</t>
-        </is>
+      <c r="A10">
+        <f>IF(Subject_Input!A9&lt;&gt;"",Subject_Input!A9,"")</f>
+        <v/>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>T10</t>
-        </is>
+      <c r="A11">
+        <f>IF(Subject_Input!A10&lt;&gt;"",Subject_Input!A10,"")</f>
+        <v/>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>T11</t>
-        </is>
+      <c r="A12">
+        <f>IF(Subject_Input!A11&lt;&gt;"",Subject_Input!A11,"")</f>
+        <v/>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>T12</t>
-        </is>
+      <c r="A13">
+        <f>IF(Subject_Input!A12&lt;&gt;"",Subject_Input!A12,"")</f>
+        <v/>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>T13</t>
-        </is>
+      <c r="A14">
+        <f>IF(Subject_Input!A13&lt;&gt;"",Subject_Input!A13,"")</f>
+        <v/>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>T14</t>
-        </is>
+      <c r="A15">
+        <f>IF(Subject_Input!A14&lt;&gt;"",Subject_Input!A14,"")</f>
+        <v/>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>T15</t>
-        </is>
+      <c r="A16">
+        <f>IF(Subject_Input!A15&lt;&gt;"",Subject_Input!A15,"")</f>
+        <v/>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>T16</t>
-        </is>
+      <c r="A17">
+        <f>IF(Subject_Input!A16&lt;&gt;"",Subject_Input!A16,"")</f>
+        <v/>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>T17</t>
-        </is>
+      <c r="A18">
+        <f>IF(Subject_Input!A17&lt;&gt;"",Subject_Input!A17,"")</f>
+        <v/>
+      </c>
+      <c r="B18" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>T18</t>
-        </is>
+      <c r="A19">
+        <f>IF(Subject_Input!A18&lt;&gt;"",Subject_Input!A18,"")</f>
+        <v/>
+      </c>
+      <c r="B19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>T19</t>
-        </is>
+      <c r="A20">
+        <f>IF(Subject_Input!A19&lt;&gt;"",Subject_Input!A19,"")</f>
+        <v/>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>T20</t>
-        </is>
+      <c r="A21">
+        <f>IF(Subject_Input!A20&lt;&gt;"",Subject_Input!A20,"")</f>
+        <v/>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>T21</t>
-        </is>
+      <c r="A22">
+        <f>IF(Subject_Input!A21&lt;&gt;"",Subject_Input!A21,"")</f>
+        <v/>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>T22</t>
-        </is>
+      <c r="A23">
+        <f>IF(Subject_Input!A22&lt;&gt;"",Subject_Input!A22,"")</f>
+        <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>T23</t>
-        </is>
+      <c r="A24">
+        <f>IF(Subject_Input!A23&lt;&gt;"",Subject_Input!A23,"")</f>
+        <v/>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>T24</t>
-        </is>
+      <c r="A25">
+        <f>IF(Subject_Input!A24&lt;&gt;"",Subject_Input!A24,"")</f>
+        <v/>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>T25</t>
-        </is>
+      <c r="A26">
+        <f>IF(Subject_Input!A25&lt;&gt;"",Subject_Input!A25,"")</f>
+        <v/>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>T26</t>
-        </is>
+      <c r="A27">
+        <f>IF(Subject_Input!A26&lt;&gt;"",Subject_Input!A26,"")</f>
+        <v/>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>T27</t>
-        </is>
+      <c r="A28">
+        <f>IF(Subject_Input!A27&lt;&gt;"",Subject_Input!A27,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <f>IF(Subject_Input!A28&lt;&gt;"",Subject_Input!A28,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <f>IF(Subject_Input!A29&lt;&gt;"",Subject_Input!A29,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <f>IF(Subject_Input!A30&lt;&gt;"",Subject_Input!A30,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <f>IF(Subject_Input!A31&lt;&gt;"",Subject_Input!A31,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <f>IF(Subject_Input!A32&lt;&gt;"",Subject_Input!A32,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <f>IF(Subject_Input!A33&lt;&gt;"",Subject_Input!A33,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <f>IF(Subject_Input!A34&lt;&gt;"",Subject_Input!A34,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <f>IF(Subject_Input!A35&lt;&gt;"",Subject_Input!A35,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <f>IF(Subject_Input!A36&lt;&gt;"",Subject_Input!A36,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <f>IF(Subject_Input!A37&lt;&gt;"",Subject_Input!A37,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <f>IF(Subject_Input!A38&lt;&gt;"",Subject_Input!A38,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <f>IF(Subject_Input!A39&lt;&gt;"",Subject_Input!A39,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <f>IF(Subject_Input!A40&lt;&gt;"",Subject_Input!A40,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <f>IF(Subject_Input!A41&lt;&gt;"",Subject_Input!A41,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <f>IF(Subject_Input!A42&lt;&gt;"",Subject_Input!A42,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <f>IF(Subject_Input!A43&lt;&gt;"",Subject_Input!A43,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <f>IF(Subject_Input!A44&lt;&gt;"",Subject_Input!A44,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <f>IF(Subject_Input!A45&lt;&gt;"",Subject_Input!A45,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <f>IF(Subject_Input!A46&lt;&gt;"",Subject_Input!A46,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <f>IF(Subject_Input!A47&lt;&gt;"",Subject_Input!A47,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <f>IF(Subject_Input!A48&lt;&gt;"",Subject_Input!A48,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <f>IF(Subject_Input!A49&lt;&gt;"",Subject_Input!A49,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <f>IF(Subject_Input!A50&lt;&gt;"",Subject_Input!A50,"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -3817,7 +4082,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -4335,203 +4600,203 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
-      <c r="B16" s="4" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="C16" s="3" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr">
+      <c r="D16" s="3" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="E16" s="3" t="inlineStr">
         <is>
           <t>h/c</t>
         </is>
       </c>
-      <c r="F16" s="4" t="inlineStr">
+      <c r="F16" s="3" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="G16" s="4" t="inlineStr">
+      <c r="G16" s="3" t="inlineStr">
         <is>
           <t>cs</t>
         </is>
       </c>
-      <c r="H16" s="4" t="inlineStr">
+      <c r="H16" s="3" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="D17" s="3" t="inlineStr">
         <is>
           <t>b</t>
         </is>
       </c>
-      <c r="E17" s="4" t="inlineStr">
+      <c r="E17" s="3" t="inlineStr">
         <is>
           <t>h/c</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" s="3" t="inlineStr">
         <is>
           <t>pe</t>
         </is>
       </c>
-      <c r="G17" s="4" t="inlineStr">
+      <c r="G17" s="3" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="4" t="inlineStr">
+      <c r="A18" s="3" t="n"/>
+      <c r="B18" s="3" t="n"/>
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
-      <c r="D18" s="4" t="inlineStr">
+      <c r="D18" s="3" t="inlineStr">
         <is>
           <t>b</t>
         </is>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="E18" s="3" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
-      <c r="F18" s="4" t="inlineStr">
+      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="G18" s="4" t="inlineStr">
+      <c r="G18" s="3" t="inlineStr">
         <is>
           <t>pe</t>
         </is>
       </c>
-      <c r="H18" s="4" t="inlineStr">
+      <c r="H18" s="3" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="D19" s="4" t="inlineStr">
+      <c r="D19" s="3" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
+      <c r="G19" s="3" t="inlineStr">
         <is>
           <t>cs</t>
         </is>
       </c>
-      <c r="H19" s="4" t="inlineStr">
+      <c r="H19" s="3" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="inlineStr">
+      <c r="A20" s="4" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="B20" s="5" t="inlineStr">
+      <c r="B20" s="4" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="C20" s="5" t="inlineStr">
+      <c r="C20" s="4" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="D20" s="5" t="inlineStr">
+      <c r="D20" s="4" t="inlineStr">
         <is>
           <t>b</t>
         </is>
       </c>
-      <c r="E20" s="5" t="inlineStr">
+      <c r="E20" s="4" t="inlineStr">
         <is>
           <t>h/c</t>
         </is>
       </c>
-      <c r="F20" s="5" t="inlineStr">
+      <c r="F20" s="4" t="inlineStr">
         <is>
           <t>cs</t>
         </is>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H20" s="5" t="inlineStr">
+      <c r="H20" s="4" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="n"/>
+      <c r="A22" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Data and main
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Classes" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -469,10 +469,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -495,8 +495,8 @@
     <col width="10.140625" bestFit="1" customWidth="1" style="1" min="16" max="16"/>
     <col width="11.140625" bestFit="1" customWidth="1" style="1" min="17" max="17"/>
     <col width="13.7109375" bestFit="1" customWidth="1" style="1" min="18" max="18"/>
-    <col width="9.140625" customWidth="1" style="1" min="19" max="26"/>
-    <col width="9.140625" customWidth="1" style="1" min="27" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="19" max="43"/>
+    <col width="9.140625" customWidth="1" style="1" min="44" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="11">
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>140001</t>
+          <t>100001</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>130001</t>
+          <t>110001</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1628,208 +1628,268 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Lib</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>140001</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>T24</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Phy</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>040102</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>T30</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Phy</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>040202</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>T57</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>130001</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>T34</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>His</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>050101</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>T40</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>His</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>050201</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>T60</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>Art</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Primary</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>120001</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>T24</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Phy</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>T35</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>His</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>Middle</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>040102</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>T30</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Phy</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>050102</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>T41</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>His</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>02</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>040202</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>T34</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>His</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>050101</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>T40</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>His</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>050201</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>T35</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>His</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>050102</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>T41</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>His</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
       <c r="R16" t="inlineStr">
         <is>
           <t>050202</t>
@@ -1837,6 +1897,36 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>T63</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>200001</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>T36</t>
@@ -2092,12 +2182,12 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2112,7 +2202,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>140101</t>
+          <t>100101</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -2154,12 +2244,12 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2174,7 +2264,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>130101</t>
+          <t>110101</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2216,12 +2306,12 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Lib</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2236,7 +2326,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>120101</t>
+          <t>140101</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2246,12 +2336,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2266,14 +2356,14 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>140201</t>
+          <t>100201</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="G24" t="inlineStr">
         <is>
-          <t>T49</t>
+          <t>T58</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2308,12 +2398,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2328,56 +2418,56 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>130201</t>
+          <t>110201</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="G25" t="inlineStr">
         <is>
-          <t>T49</t>
+          <t>T61</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>120101</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>T56</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
           <t>Lib</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="O25" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>140101</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>T56</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>Art</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
       <c r="P25" t="inlineStr">
         <is>
           <t>Secondary</t>
@@ -2390,24 +2480,24 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>120201</t>
+          <t>140201</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="G26" t="inlineStr">
         <is>
-          <t>T46</t>
+          <t>T64</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>20</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2422,7 +2512,101 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>140101</t>
+          <t>200101</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>T59</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>130201</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>T62</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>120201</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>T65</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>200201</t>
         </is>
       </c>
     </row>
@@ -2443,10 +2627,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3280,7 +3464,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3297,7 +3481,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3314,7 +3498,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3331,7 +3515,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3348,7 +3532,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3365,7 +3549,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3382,7 +3566,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Lib</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3399,7 +3583,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Lib</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3416,16 +3600,169 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>Lib</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>T57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>T58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>T59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>T60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>Art</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-    </row>
-    <row r="58"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>T61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>T62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>T63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>T64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>T65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="67"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3441,7 +3778,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3523,7 +3860,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Iind Lang</t>
+          <t>IInd Lang</t>
         </is>
       </c>
     </row>
@@ -3609,10 +3946,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3620,6 +3957,7 @@
     <col width="7.85546875" bestFit="1" customWidth="1" style="13" min="2" max="2"/>
     <col width="7.28515625" customWidth="1" style="13" min="3" max="3"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
+    <col width="11" customWidth="1" style="13" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3628,6 +3966,11 @@
           <t>Max Lectures/Week</t>
         </is>
       </c>
+      <c r="E1" s="12" t="inlineStr">
+        <is>
+          <t>Max Lectures/Day</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="13">
       <c r="A2" s="7" t="inlineStr">
@@ -3650,11 +3993,27 @@
           <t>Secondary</t>
         </is>
       </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <f>IF(Subject_Input!A2&lt;&gt;"",Subject_Input!A2,"")</f>
-        <v/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>7</v>
@@ -3665,11 +4024,21 @@
       <c r="D3" t="n">
         <v>6</v>
       </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <f>IF(Subject_Input!A3&lt;&gt;"",Subject_Input!A3,"")</f>
-        <v/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bio</t>
+        </is>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -3677,11 +4046,18 @@
       <c r="D4" t="n">
         <v>3</v>
       </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <f>IF(Subject_Input!A4&lt;&gt;"",Subject_Input!A4,"")</f>
-        <v/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Chem</t>
+        </is>
       </c>
       <c r="C5" t="n">
         <v>3</v>
@@ -3689,11 +4065,18 @@
       <c r="D5" t="n">
         <v>3</v>
       </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <f>IF(Subject_Input!A5&lt;&gt;"",Subject_Input!A5,"")</f>
-        <v/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Phy</t>
+        </is>
       </c>
       <c r="C6" t="n">
         <v>3</v>
@@ -3701,11 +4084,18 @@
       <c r="D6" t="n">
         <v>3</v>
       </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <f>IF(Subject_Input!A6&lt;&gt;"",Subject_Input!A6,"")</f>
-        <v/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>His</t>
+        </is>
       </c>
       <c r="C7" t="n">
         <v>2</v>
@@ -3713,11 +4103,18 @@
       <c r="D7" t="n">
         <v>2</v>
       </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <f>IF(Subject_Input!A7&lt;&gt;"",Subject_Input!A7,"")</f>
-        <v/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Civ</t>
+        </is>
       </c>
       <c r="C8" t="n">
         <v>2</v>
@@ -3725,11 +4122,18 @@
       <c r="D8" t="n">
         <v>2</v>
       </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <f>IF(Subject_Input!A8&lt;&gt;"",Subject_Input!A8,"")</f>
-        <v/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Geo</t>
+        </is>
       </c>
       <c r="C9" t="n">
         <v>2</v>
@@ -3737,20 +4141,31 @@
       <c r="D9" t="n">
         <v>2</v>
       </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <f>IF(Subject_Input!A9&lt;&gt;"",Subject_Input!A9,"")</f>
-        <v/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Eco</t>
+        </is>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <f>IF(Subject_Input!A10&lt;&gt;"",Subject_Input!A10,"")</f>
-        <v/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Eng</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>5</v>
@@ -3761,11 +4176,21 @@
       <c r="D11" t="n">
         <v>5</v>
       </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12">
-        <f>IF(Subject_Input!A11&lt;&gt;"",Subject_Input!A11,"")</f>
-        <v/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>IInd Lang</t>
+        </is>
       </c>
       <c r="C12" t="n">
         <v>3</v>
@@ -3773,11 +4198,18 @@
       <c r="D12" t="n">
         <v>5</v>
       </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13">
-        <f>IF(Subject_Input!A12&lt;&gt;"",Subject_Input!A12,"")</f>
-        <v/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Pe</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>2</v>
@@ -3788,11 +4220,21 @@
       <c r="D13" t="n">
         <v>2</v>
       </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14">
-        <f>IF(Subject_Input!A13&lt;&gt;"",Subject_Input!A13,"")</f>
-        <v/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -3803,11 +4245,21 @@
       <c r="D14" t="n">
         <v>1</v>
       </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15">
-        <f>IF(Subject_Input!A14&lt;&gt;"",Subject_Input!A14,"")</f>
-        <v/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
       </c>
       <c r="C15" t="n">
         <v>1</v>
@@ -3815,11 +4267,18 @@
       <c r="D15" t="n">
         <v>1</v>
       </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16">
-        <f>IF(Subject_Input!A15&lt;&gt;"",Subject_Input!A15,"")</f>
-        <v/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Lib</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -3830,29 +4289,47 @@
       <c r="D16" t="n">
         <v>1</v>
       </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17">
-        <f>IF(Subject_Input!A16&lt;&gt;"",Subject_Input!A16,"")</f>
-        <v/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SST</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>5</v>
       </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18">
-        <f>IF(Subject_Input!A17&lt;&gt;"",Subject_Input!A17,"")</f>
-        <v/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Science</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>5</v>
       </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19">
-        <f>IF(Subject_Input!A18&lt;&gt;"",Subject_Input!A18,"")</f>
-        <v/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hindi</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>5</v>
@@ -3860,29 +4337,44 @@
       <c r="C19" t="n">
         <v>3</v>
       </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20">
-        <f>IF(Subject_Input!A19&lt;&gt;"",Subject_Input!A19,"")</f>
-        <v/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Marathi</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>2</v>
       </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21">
-        <f>IF(Subject_Input!A20&lt;&gt;"",Subject_Input!A20,"")</f>
-        <v/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GK</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>2</v>
       </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22">
-        <f>IF(Subject_Input!A21&lt;&gt;"",Subject_Input!A21,"")</f>
-        <v/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>3</v>
@@ -3890,184 +4382,23 @@
       <c r="C22" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <f>IF(Subject_Input!A22&lt;&gt;"",Subject_Input!A22,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <f>IF(Subject_Input!A23&lt;&gt;"",Subject_Input!A23,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <f>IF(Subject_Input!A24&lt;&gt;"",Subject_Input!A24,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <f>IF(Subject_Input!A25&lt;&gt;"",Subject_Input!A25,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <f>IF(Subject_Input!A26&lt;&gt;"",Subject_Input!A26,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <f>IF(Subject_Input!A27&lt;&gt;"",Subject_Input!A27,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <f>IF(Subject_Input!A28&lt;&gt;"",Subject_Input!A28,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <f>IF(Subject_Input!A29&lt;&gt;"",Subject_Input!A29,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <f>IF(Subject_Input!A30&lt;&gt;"",Subject_Input!A30,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <f>IF(Subject_Input!A31&lt;&gt;"",Subject_Input!A31,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <f>IF(Subject_Input!A32&lt;&gt;"",Subject_Input!A32,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <f>IF(Subject_Input!A33&lt;&gt;"",Subject_Input!A33,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <f>IF(Subject_Input!A34&lt;&gt;"",Subject_Input!A34,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36">
-        <f>IF(Subject_Input!A35&lt;&gt;"",Subject_Input!A35,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37">
-        <f>IF(Subject_Input!A36&lt;&gt;"",Subject_Input!A36,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38">
-        <f>IF(Subject_Input!A37&lt;&gt;"",Subject_Input!A37,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39">
-        <f>IF(Subject_Input!A38&lt;&gt;"",Subject_Input!A38,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40">
-        <f>IF(Subject_Input!A39&lt;&gt;"",Subject_Input!A39,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <f>IF(Subject_Input!A40&lt;&gt;"",Subject_Input!A40,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <f>IF(Subject_Input!A41&lt;&gt;"",Subject_Input!A41,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <f>IF(Subject_Input!A42&lt;&gt;"",Subject_Input!A42,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <f>IF(Subject_Input!A43&lt;&gt;"",Subject_Input!A43,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <f>IF(Subject_Input!A44&lt;&gt;"",Subject_Input!A44,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <f>IF(Subject_Input!A45&lt;&gt;"",Subject_Input!A45,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <f>IF(Subject_Input!A46&lt;&gt;"",Subject_Input!A46,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <f>IF(Subject_Input!A47&lt;&gt;"",Subject_Input!A47,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <f>IF(Subject_Input!A48&lt;&gt;"",Subject_Input!A48,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <f>IF(Subject_Input!A49&lt;&gt;"",Subject_Input!A49,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <f>IF(Subject_Input!A50&lt;&gt;"",Subject_Input!A50,"")</f>
-        <v/>
+      <c r="D22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated main.py and Data.xlsx
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
@@ -495,8 +495,8 @@
     <col width="10.140625" bestFit="1" customWidth="1" style="1" min="16" max="16"/>
     <col width="11.140625" bestFit="1" customWidth="1" style="1" min="17" max="17"/>
     <col width="13.7109375" bestFit="1" customWidth="1" style="1" min="18" max="18"/>
-    <col width="9.140625" customWidth="1" style="1" min="19" max="43"/>
-    <col width="9.140625" customWidth="1" style="1" min="44" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="19" max="47"/>
+    <col width="9.140625" customWidth="1" style="1" min="48" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="11">
@@ -671,7 +671,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>T7</t>
+          <t>T8</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>T8</t>
+          <t>T9</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>T9</t>
+          <t>T10</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -887,7 +887,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>T10</t>
+          <t>T11</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -917,17 +917,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>T13</t>
+          <t>T7</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Eng</t>
+          <t>Maths</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>01</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -942,12 +942,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>090101</t>
+          <t>010104</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>T16</t>
+          <t>T18</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -979,7 +979,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T11</t>
+          <t>T12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1034,12 +1034,12 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>090102</t>
+          <t>090101</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>T17</t>
+          <t>T19</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1071,7 +1071,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>T12</t>
+          <t>T13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1126,12 +1126,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>090103</t>
+          <t>090102</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>T18</t>
+          <t>T20</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1163,7 +1163,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>T31</t>
+          <t>T38</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1193,69 +1193,69 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>T19</t>
+          <t>T16</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Bio</t>
+          <t>Eng</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>090103</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>T21</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Eng</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
           <t>02</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>020101</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>T25</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Bio</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>020201</t>
+          <t>090204</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>T32</t>
+          <t>T39</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1285,69 +1285,69 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>T20</t>
+          <t>T17</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>Eng</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>090104</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>T31</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
           <t>Bio</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>02</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>020102</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>T26</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Bio</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>02</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>020202</t>
+          <t>020201</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>T33</t>
+          <t>T40</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1377,17 +1377,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>T21</t>
+          <t>T22</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Chem</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1402,22 +1402,22 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>030101</t>
+          <t>020101</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>T27</t>
+          <t>T32</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Chem</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1432,14 +1432,14 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>030201</t>
+          <t>020202</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>T48</t>
+          <t>T55</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1469,49 +1469,49 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>T22</t>
+          <t>T23</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
+          <t>Bio</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>020102</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>T33</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
           <t>Chem</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>03</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>030102</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>T28</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>Chem</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
       <c r="P12" t="inlineStr">
         <is>
           <t>Secondary</t>
@@ -1524,14 +1524,14 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>030202</t>
+          <t>030201</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>T51</t>
+          <t>T61</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1561,17 +1561,17 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>T23</t>
+          <t>T24</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Phy</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>02</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1586,22 +1586,22 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>040101</t>
+          <t>020103</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>T29</t>
+          <t>T34</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Phy</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1616,14 +1616,14 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>040201</t>
+          <t>030202</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>T54</t>
+          <t>T64</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1653,17 +1653,17 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>T24</t>
+          <t>T25</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Phy</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1678,22 +1678,22 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>040102</t>
+          <t>030101</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>T30</t>
+          <t>T35</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Phy</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1708,14 +1708,14 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>040202</t>
+          <t>030203</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T57</t>
+          <t>T67</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1745,17 +1745,17 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>T34</t>
+          <t>T26</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>03</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1770,22 +1770,22 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>050101</t>
+          <t>030102</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>T40</t>
+          <t>T36</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1800,14 +1800,14 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>050201</t>
+          <t>040201</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T60</t>
+          <t>T70</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1837,17 +1837,17 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>T35</t>
+          <t>T27</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>03</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1862,22 +1862,22 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>050102</t>
+          <t>030103</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>T41</t>
+          <t>T37</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1892,14 +1892,14 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>050202</t>
+          <t>040202</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>T63</t>
+          <t>T73</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1929,17 +1929,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>T36</t>
+          <t>T28</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>04</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1954,22 +1954,22 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>060101</t>
+          <t>040101</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>T42</t>
+          <t>T47</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>His</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1984,24 +1984,24 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>060201</t>
+          <t>050201</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="G18" t="inlineStr">
         <is>
-          <t>T37</t>
+          <t>T29</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>04</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2016,22 +2016,22 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>060102</t>
+          <t>040102</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>T43</t>
+          <t>T48</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>His</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2046,24 +2046,24 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>060202</t>
+          <t>050202</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="G19" t="inlineStr">
         <is>
-          <t>T38</t>
+          <t>T30</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>04</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2078,22 +2078,22 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>070101</t>
+          <t>040103</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>T44</t>
+          <t>T49</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>Civ</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2108,24 +2108,24 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>070201</t>
+          <t>060201</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="G20" t="inlineStr">
         <is>
-          <t>T39</t>
+          <t>T41</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>His</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>05</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2140,22 +2140,22 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>070102</t>
+          <t>050101</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>T45</t>
+          <t>T50</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>Civ</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2170,24 +2170,24 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>070202</t>
+          <t>060202</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="G21" t="inlineStr">
         <is>
-          <t>T49</t>
+          <t>T42</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>IInd Lang</t>
+          <t>His</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>05</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2202,22 +2202,22 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>100101</t>
+          <t>050102</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>T46</t>
+          <t>T51</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Eco</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2232,54 +2232,54 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>080201</t>
+          <t>070201</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="G22" t="inlineStr">
         <is>
+          <t>T43</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Civ</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>060101</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
           <t>T52</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Pe</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>110101</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>T47</t>
-        </is>
-      </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Eco</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2294,24 +2294,24 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>080202</t>
+          <t>070202</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="G23" t="inlineStr">
         <is>
-          <t>T55</t>
+          <t>T44</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>Civ</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>06</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2326,22 +2326,22 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>140101</t>
+          <t>060102</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>T50</t>
+          <t>T53</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>IInd Lang</t>
+          <t>Eco</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>08</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2356,24 +2356,24 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>100201</t>
+          <t>080201</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="G24" t="inlineStr">
         <is>
-          <t>T58</t>
+          <t>T45</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>07</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2388,22 +2388,22 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>130101</t>
+          <t>070101</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>T53</t>
+          <t>T54</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Pe</t>
+          <t>Eco</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>08</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2418,24 +2418,24 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>110201</t>
+          <t>080202</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="G25" t="inlineStr">
         <is>
-          <t>T61</t>
+          <t>T46</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>07</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2450,22 +2450,22 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>120101</t>
+          <t>070102</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>T56</t>
+          <t>T59</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2480,133 +2480,443 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>140201</t>
+          <t>100201</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="G26" t="inlineStr">
         <is>
-          <t>T64</t>
+          <t>T56</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>IInd Lang</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>100101</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>T60</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>IInd Lang</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>100202</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>T57</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>IInd Lang</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>100102</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>T63</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Pe</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>110201</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>T58</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>IInd Lang</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>100103</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>T66</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Lib</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>140201</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>T62</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Pe</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>110101</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>T69</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>130201</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>T65</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Lib</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>140101</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>T72</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>120201</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>T68</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>130101</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>T75</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
           <t>CS</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="O31" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>200201</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>T71</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>120101</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>T74</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>200101</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>T59</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>Yoga</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>130201</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>T62</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>Art</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>120201</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>T65</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>200201</t>
         </is>
       </c>
     </row>
@@ -2627,10 +2937,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:A66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2742,7 +3052,7 @@
         </is>
       </c>
     </row>
-    <row r="7">
+    <row r="7" s="13">
       <c r="A7" t="inlineStr">
         <is>
           <t>T6</t>
@@ -2772,7 +3082,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -2818,12 +3128,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Eng</t>
+          <t>Maths</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -2874,7 +3184,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -2912,7 +3222,7 @@
         </is>
       </c>
     </row>
-    <row r="17">
+    <row r="17" s="13">
       <c r="A17" t="inlineStr">
         <is>
           <t>T16</t>
@@ -2925,7 +3235,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -2942,7 +3252,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -2971,12 +3281,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bio</t>
+          <t>Eng</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -2988,12 +3298,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bio</t>
+          <t>Eng</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3315,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Chem</t>
+          <t>Eng</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3022,7 +3332,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Chem</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -3031,7 +3341,7 @@
         </is>
       </c>
     </row>
-    <row r="24">
+    <row r="24" s="13">
       <c r="A24" t="inlineStr">
         <is>
           <t>T23</t>
@@ -3039,7 +3349,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Phy</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3056,7 +3366,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Phy</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3073,16 +3383,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bio</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" s="13">
       <c r="A27" t="inlineStr">
         <is>
           <t>T26</t>
@@ -3090,12 +3400,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bio</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3112,7 +3422,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3124,16 +3434,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Chem</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" s="13">
       <c r="A30" t="inlineStr">
         <is>
           <t>T29</t>
@@ -3146,7 +3456,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3473,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3485,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3192,12 +3502,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3209,12 +3519,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3226,12 +3536,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3243,12 +3553,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>Chem</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3570,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3277,12 +3587,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>Phy</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3294,12 +3604,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>SST</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -3311,12 +3621,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>SST</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -3328,12 +3638,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>His</t>
+          <t>SST</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3660,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3362,12 +3672,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Civ</t>
+          <t>His</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3384,7 +3694,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3396,12 +3706,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Geo</t>
+          <t>Civ</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3418,7 +3728,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3740,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Eco</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3447,7 +3757,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Eco</t>
+          <t>His</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3464,12 +3774,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>IInd Lang</t>
+          <t>His</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3481,12 +3791,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>IInd Lang</t>
+          <t>Civ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3498,7 +3808,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>IInd Lang</t>
+          <t>Civ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3515,12 +3825,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Pe</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3532,12 +3842,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Pe</t>
+          <t>Geo</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3549,7 +3859,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Pe</t>
+          <t>Eco</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3566,12 +3876,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>Eco</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3583,12 +3893,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -3600,16 +3910,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Lib</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" s="13">
       <c r="A58" t="inlineStr">
         <is>
           <t>T57</t>
@@ -3617,16 +3927,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Primary</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" s="13">
       <c r="A59" t="inlineStr">
         <is>
           <t>T58</t>
@@ -3634,7 +3944,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3651,7 +3961,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Yoga</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3668,12 +3978,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>IInd Lang</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3685,12 +3995,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -3702,12 +4012,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Secondary</t>
+          <t>Middle</t>
         </is>
       </c>
     </row>
@@ -3719,12 +4029,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>Pe</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Primary</t>
+          <t>Secondary</t>
         </is>
       </c>
     </row>
@@ -3736,12 +4046,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>Lib</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Primary</t>
         </is>
       </c>
     </row>
@@ -3753,16 +4063,186 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>Lib</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>T66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Lib</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>T67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>T68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>T69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>T70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>T71</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>T72</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>T73</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>CS</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Secondary</t>
-        </is>
-      </c>
-    </row>
-    <row r="67"/>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>T74</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>T75</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Secondary</t>
+        </is>
+      </c>
+    </row>
+    <row r="77"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3777,7 +4257,7 @@
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3949,7 +4429,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4022,7 +4502,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -4174,7 +4654,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>

</xml_diff>